<commit_message>
Se agraga el Proyecto
</commit_message>
<xml_diff>
--- a/Porticos 2D/vigas winkler/resultados.xlsx
+++ b/Porticos 2D/vigas winkler/resultados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Poli\ELEMENTOS FINITOS\Elementos finitos_1\Porticos 2D\vigas winkler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C06FF029-071E-4642-A5CE-ECF3D2C100AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989D210-41F5-4AC4-8942-DE7A5C8A1C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0AE346B2-6587-44B7-80A4-1C07BE948755}"/>
   </bookViews>
@@ -37,6 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -120,6 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,13 +236,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>145360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>199524</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>132925</xdr:rowOff>
+      <xdr:rowOff>116360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -261,7 +265,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2828925"/>
+          <a:off x="0" y="1669360"/>
           <a:ext cx="4009524" cy="3400000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -703,15 +707,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0D446B-1E77-4B3E-BE37-E350AB2446A9}">
-  <dimension ref="A2:K10"/>
+  <dimension ref="A2:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -723,8 +727,46 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
+      <c r="L2">
+        <v>994802.49199999997</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>-994802.49199999997</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>+A3-L2</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="9">
+        <f t="shared" ref="S2:U7" si="0">+B3-M2</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U2" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V2" s="9">
+        <f t="shared" ref="V2:V7" si="1">+E3-P2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>994802.49199999997</v>
       </c>
@@ -746,8 +788,46 @@
       <c r="G3">
         <v>53.333333333330998</v>
       </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>10396.6123624712</v>
+      </c>
+      <c r="N3">
+        <v>19730.882009283301</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>-9400.4451619573701</v>
+      </c>
+      <c r="Q3">
+        <v>19067.4719243488</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" ref="R3:R7" si="2">+A4-L3</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V3" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -769,8 +849,46 @@
       <c r="G4">
         <v>52.799793240196301</v>
       </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>19730.882009283301</v>
+      </c>
+      <c r="N4">
+        <v>52198.298924370101</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>-19067.4719243488</v>
+      </c>
+      <c r="Q4">
+        <v>25139.677461503899</v>
+      </c>
+      <c r="R4" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -792,8 +910,46 @@
       <c r="G5" s="7">
         <v>35.840725967924399</v>
       </c>
+      <c r="L5">
+        <v>-994802.49199999997</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>994802.49199999997</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-994802.49199999997</v>
       </c>
@@ -815,8 +971,46 @@
       <c r="G6">
         <v>56.666666666669798</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>-9400.4451619573701</v>
+      </c>
+      <c r="N6">
+        <v>-19067.4719243488</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>10396.6123624712</v>
+      </c>
+      <c r="Q6">
+        <v>-19730.882009283301</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -839,8 +1033,50 @@
         <v>56.778598816328298</v>
       </c>
       <c r="K7" s="7"/>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>19067.4719243488</v>
+      </c>
+      <c r="N7">
+        <v>25139.677461503899</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>-19730.882009283301</v>
+      </c>
+      <c r="Q7">
+        <v>52198.298924370101</v>
+      </c>
+      <c r="R7" s="9">
+        <f>+A8-L7</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="9">
+        <f>+B8-M7</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="9">
+        <f>+D8-O7</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="9">
+        <f>+F8-Q7</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -863,7 +1099,7 @@
         <v>-37.134383374878503</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K10" s="7"/>
     </row>
   </sheetData>

</xml_diff>